<commit_message>
Test data updated 4/21
</commit_message>
<xml_diff>
--- a/JDA_SOQ_Automation/src/test/java/testData/SOQDataSheet.xlsx
+++ b/JDA_SOQ_Automation/src/test/java/testData/SOQDataSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FD4210-A999-4126-9F2E-BF42C2A8A9A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24D332F-62BC-4CE5-ACB4-9381CE72FEAF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -699,7 +699,7 @@
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,8 +718,8 @@
     <col min="13" max="13" width="11.140625" style="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="10.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="14.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="29.140625" style="1" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="51.42578125" style="1" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="29.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="51.42578125" style="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="21" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="22" max="16384" width="9.140625" style="1" collapsed="1"/>
@@ -811,7 +811,7 @@
         <v>43942</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>17</v>
@@ -834,13 +834,13 @@
       <c r="N2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="6" t="e">
-        <f>CONCATENATE(#REF!,D2,TEXT(K2,"mm/dd/yy"),O2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q2" s="6" t="e">
-        <f>CONCATENATE(#REF!,D2)</f>
-        <v>#REF!</v>
+      <c r="P2" s="6" t="str">
+        <f>CONCATENATE(C2,D2,TEXT(K2,"mm/dd/yy"),O2)</f>
+        <v>4460998701-100004/29/20</v>
+      </c>
+      <c r="Q2" s="6" t="str">
+        <f>CONCATENATE(P2,G2)</f>
+        <v>4460998701-100004/29/20BA</v>
       </c>
       <c r="R2" s="15">
         <v>43942</v>
@@ -871,7 +871,7 @@
         <v>43942</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>17</v>
@@ -894,13 +894,13 @@
       <c r="N3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="6" t="e">
-        <f>CONCATENATE(#REF!,D3,TEXT(K3,"mm/dd/yy"),O3)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q3" s="6" t="e">
-        <f>CONCATENATE(#REF!,D3)</f>
-        <v>#REF!</v>
+      <c r="P3" s="6" t="str">
+        <f>CONCATENATE(C3,D3,TEXT(K3,"mm/dd/yy"),O3)</f>
+        <v>4058988701-100004/29/20</v>
+      </c>
+      <c r="Q3" s="6" t="str">
+        <f>CONCATENATE(P3,G3)</f>
+        <v>4058988701-100004/29/20HO</v>
       </c>
       <c r="R3" s="15">
         <v>43942</v>

</xml_diff>